<commit_message>
modify test spec for algieba
</commit_message>
<xml_diff>
--- a/algieba/test/function_test.xlsx
+++ b/algieba/test/function_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="179">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -1421,82 +1421,7 @@
   <si>
     <t>status: bad_request
 body: [
-  {error_code: absent_param_account_type},
-  {error_code: absent_param_date},
-  {error_code: absent_param_content},
-  {error_code: absent_param_category},
-  {error_code: absent_param_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
   {error_code: absent_param_accounts}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_date}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_account_type},
-  {error_code: invalid_value_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_date}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_with},
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1504,20 +1429,6 @@
     <t>status: bad_request
 body: [
   {error_code: absent_param_with}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_value_interval}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1829,6 +1740,56 @@
     <rPh sb="11" eb="13">
       <t>キノウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: absent_param_accounts}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: absent_param_with},
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_param_account_type}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_param_date}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_param_price}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_param_account_type},
+  {error_code: invalid_param_price}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_param_interval}
+]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3054,10 +3015,10 @@
         <v>53</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="31">
@@ -3120,7 +3081,7 @@
         <v>76</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>53</v>
@@ -3143,7 +3104,7 @@
         <v>76</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>53</v>
@@ -3189,7 +3150,7 @@
         <v>76</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>53</v>
@@ -3284,7 +3245,7 @@
         <v>53</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="H13" s="45" t="s">
         <v>112</v>
@@ -3307,7 +3268,7 @@
         <v>56</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="H14" s="45" t="s">
         <v>112</v>
@@ -3422,7 +3383,7 @@
         <v>56</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>112</v>
@@ -3583,7 +3544,7 @@
         <v>53</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>113</v>
@@ -3606,7 +3567,7 @@
         <v>59</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="H27" s="47" t="s">
         <v>113</v>
@@ -3766,8 +3727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3820,7 +3781,7 @@
         <v>53</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="H3" s="44" t="s">
         <v>142</v>
@@ -3843,7 +3804,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H4" s="45" t="s">
         <v>143</v>
@@ -3866,7 +3827,7 @@
         <v>69</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="H5" s="46" t="s">
         <v>144</v>
@@ -3889,7 +3850,7 @@
         <v>53</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="H6" s="46" t="s">
         <v>145</v>
@@ -3912,7 +3873,7 @@
         <v>53</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="H7" s="46" t="s">
         <v>146</v>
@@ -3935,13 +3896,13 @@
         <v>53</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="H8" s="46" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="109">
+    <row r="9" spans="2:8" ht="57">
       <c r="B9" s="21">
         <v>7</v>
       </c>
@@ -3961,7 +3922,7 @@
         <v>116</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="57">
@@ -3984,7 +3945,7 @@
         <v>106</v>
       </c>
       <c r="H10" s="46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="96">
@@ -4004,10 +3965,10 @@
         <v>53</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="H11" s="45" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="96">
@@ -4027,10 +3988,10 @@
         <v>71</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="96">
@@ -4050,10 +4011,10 @@
         <v>70</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="96">
@@ -4073,10 +4034,10 @@
         <v>72</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="57">
@@ -4099,7 +4060,7 @@
         <v>53</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="57">
@@ -4122,7 +4083,7 @@
         <v>73</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="57">
@@ -4145,7 +4106,7 @@
         <v>53</v>
       </c>
       <c r="H17" s="45" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="83">
@@ -4168,7 +4129,7 @@
         <v>122</v>
       </c>
       <c r="H18" s="45" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="83">
@@ -4191,7 +4152,7 @@
         <v>123</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="83">
@@ -4214,7 +4175,7 @@
         <v>141</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="57">
@@ -4237,7 +4198,7 @@
         <v>124</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="57">
@@ -4260,7 +4221,7 @@
         <v>125</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="57">
@@ -4283,7 +4244,7 @@
         <v>126</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="57">
@@ -4306,7 +4267,7 @@
         <v>127</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="57">
@@ -4329,7 +4290,7 @@
         <v>132</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="57">
@@ -4352,7 +4313,7 @@
         <v>134</v>
       </c>
       <c r="H26" s="45" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="57">
@@ -4375,7 +4336,7 @@
         <v>135</v>
       </c>
       <c r="H27" s="45" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="57">
@@ -4395,10 +4356,10 @@
         <v>53</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="H28" s="45" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="57">
@@ -4421,7 +4382,7 @@
         <v>138</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="58" thickBot="1">
@@ -4444,7 +4405,7 @@
         <v>53</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="2:8">

</xml_diff>